<commit_message>
added rest of the data
</commit_message>
<xml_diff>
--- a/data&charts/AlgoResults.xlsx
+++ b/data&charts/AlgoResults.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derre\java\IntelliJ\github-workspace\CSB340\CSB340_CPUScheduler\src\data&amp;charts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derre\java\IntelliJ\github-workspace\CSB340\CSB340_CPUScheduler\data&amp;charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0BA18E-E061-459D-8A1C-EC7442BB96D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB6F041-D476-4027-B26E-3FAFBEC5FDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E64E7D82-C98A-4F1C-A029-AE82D3AC3812}"/>
   </bookViews>
@@ -107,15 +107,6 @@
     <t>AVG</t>
   </si>
   <si>
-    <t xml:space="preserve">RR - CPU Utilization: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Priority - CPU Utilization: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MLQ - CPU Utilization: </t>
-  </si>
-  <si>
     <t>MLFQ - CPU Utilization: 89.48%</t>
   </si>
   <si>
@@ -123,6 +114,15 @@
   </si>
   <si>
     <t>SJF - CPU Utilization: 82.8%</t>
+  </si>
+  <si>
+    <t>Priority - CPU Utilization: 83.4</t>
+  </si>
+  <si>
+    <t>MLQ - CPU Utilization: 95.8%</t>
+  </si>
+  <si>
+    <t>RR - CPU Utilization: 92.9%</t>
   </si>
 </sst>
 </file>
@@ -163,14 +163,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4CC5269-70C9-4B9F-8E51-DDEAE9BA5460}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.28515625" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -518,33 +518,51 @@
       <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>0.85340000000000005</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>0.82799999999999996</v>
       </c>
-      <c r="G2" s="3">
+      <c r="D2" s="2">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="G2" s="2">
         <v>0.89480000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1">
         <v>185.25</v>
       </c>
       <c r="C3" s="1">
         <v>133.5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>153.6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>175.9</v>
+      </c>
+      <c r="F3" s="1">
+        <v>148</v>
       </c>
       <c r="G3" s="1">
         <v>165.63</v>
@@ -560,6 +578,15 @@
       <c r="C4" s="1">
         <v>469.6</v>
       </c>
+      <c r="D4" s="1">
+        <v>489.8</v>
+      </c>
+      <c r="E4" s="1">
+        <v>512</v>
+      </c>
+      <c r="F4" s="1">
+        <v>484.1</v>
+      </c>
       <c r="G4" s="1">
         <v>501.75</v>
       </c>
@@ -574,26 +601,35 @@
       <c r="C5" s="1">
         <v>27.1</v>
       </c>
+      <c r="D5" s="1">
+        <v>49.6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>15.8</v>
+      </c>
+      <c r="F5" s="1">
+        <v>24.6</v>
+      </c>
       <c r="G5" s="1">
         <v>15.75</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="H7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="M7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="H7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="M7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -649,8 +685,26 @@
       <c r="G9" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="H9" s="1">
+        <v>117</v>
+      </c>
+      <c r="I9" s="1">
+        <v>27</v>
+      </c>
+      <c r="J9" s="1">
+        <v>342</v>
+      </c>
       <c r="L9" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="M9" s="1">
+        <v>15</v>
+      </c>
+      <c r="N9" s="1">
+        <v>240</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -669,8 +723,26 @@
       <c r="G10" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="H10" s="1">
+        <v>236</v>
+      </c>
+      <c r="I10" s="1">
+        <v>663</v>
+      </c>
+      <c r="J10" s="1">
+        <v>67</v>
+      </c>
       <c r="L10" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="M10" s="1">
+        <v>35</v>
+      </c>
+      <c r="N10" s="1">
+        <v>462</v>
+      </c>
+      <c r="O10" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -689,8 +761,26 @@
       <c r="G11" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="H11" s="1">
+        <v>113</v>
+      </c>
+      <c r="I11" s="1">
+        <v>505</v>
+      </c>
+      <c r="J11" s="1">
+        <v>35</v>
+      </c>
       <c r="L11" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="M11" s="1">
+        <v>57</v>
+      </c>
+      <c r="N11" s="1">
+        <v>449</v>
+      </c>
+      <c r="O11" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -709,8 +799,26 @@
       <c r="G12" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="H12" s="1">
+        <v>96</v>
+      </c>
+      <c r="I12" s="1">
+        <v>580</v>
+      </c>
+      <c r="J12" s="1">
+        <v>32</v>
+      </c>
       <c r="L12" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="M12" s="1">
+        <v>17</v>
+      </c>
+      <c r="N12" s="1">
+        <v>501</v>
+      </c>
+      <c r="O12" s="1">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -729,8 +837,26 @@
       <c r="G13" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H13" s="1">
+        <v>45</v>
+      </c>
+      <c r="I13" s="1">
+        <v>354</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
       <c r="L13" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="M13" s="1">
+        <v>268</v>
+      </c>
+      <c r="N13" s="1">
+        <v>577</v>
+      </c>
+      <c r="O13" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -749,8 +875,26 @@
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="H14" s="1">
+        <v>77</v>
+      </c>
+      <c r="I14" s="1">
+        <v>292</v>
+      </c>
+      <c r="J14" s="1">
+        <v>16</v>
+      </c>
       <c r="L14" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="M14" s="1">
+        <v>325</v>
+      </c>
+      <c r="N14" s="1">
+        <v>540</v>
+      </c>
+      <c r="O14" s="1">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -769,9 +913,27 @@
       <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="4"/>
+      <c r="H15" s="1">
+        <v>277</v>
+      </c>
+      <c r="I15" s="1">
+        <v>605</v>
+      </c>
+      <c r="J15" s="1">
+        <v>112</v>
+      </c>
+      <c r="K15" s="3"/>
       <c r="L15" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="M15" s="1">
+        <v>244</v>
+      </c>
+      <c r="N15" s="1">
+        <v>572</v>
+      </c>
+      <c r="O15" s="1">
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -790,8 +952,26 @@
       <c r="G16" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H16" s="1">
+        <v>268</v>
+      </c>
+      <c r="I16" s="1">
+        <v>577</v>
+      </c>
+      <c r="J16" s="1">
+        <v>108</v>
+      </c>
       <c r="L16" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="M16" s="1">
+        <v>223</v>
+      </c>
+      <c r="N16" s="1">
+        <v>532</v>
+      </c>
+      <c r="O16" s="1">
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="2:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -810,26 +990,44 @@
       <c r="G17" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="H17" s="1">
+        <v>153.6</v>
+      </c>
+      <c r="I17" s="1">
+        <v>489.8</v>
+      </c>
+      <c r="J17" s="1">
+        <v>49.6</v>
+      </c>
       <c r="L17" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="M17" s="1">
+        <v>148</v>
+      </c>
+      <c r="N17" s="1">
+        <v>584.1</v>
+      </c>
+      <c r="O17" s="1">
+        <v>24.6</v>
+      </c>
     </row>
     <row r="19" spans="2:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="H19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="M19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="M19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
     </row>
     <row r="20" spans="2:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
@@ -885,6 +1083,15 @@
       <c r="G21" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="H21" s="1">
+        <v>107</v>
+      </c>
+      <c r="I21" s="1">
+        <v>332</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
       <c r="L21" s="1" t="s">
         <v>10</v>
       </c>
@@ -903,16 +1110,25 @@
         <v>11</v>
       </c>
       <c r="C22" s="1">
-        <v>121</v>
+        <v>73</v>
       </c>
       <c r="D22" s="1">
-        <v>336</v>
+        <v>500</v>
       </c>
       <c r="E22" s="1">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="H22" s="1">
+        <v>125</v>
+      </c>
+      <c r="I22" s="1">
+        <v>552</v>
+      </c>
+      <c r="J22" s="1">
+        <v>5</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>11</v>
@@ -932,16 +1148,25 @@
         <v>12</v>
       </c>
       <c r="C23" s="1">
-        <v>119</v>
+        <v>276</v>
       </c>
       <c r="D23" s="1">
-        <v>428</v>
+        <v>668</v>
       </c>
       <c r="E23" s="1">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="H23" s="1">
+        <v>203</v>
+      </c>
+      <c r="I23" s="1">
+        <v>595</v>
+      </c>
+      <c r="J23" s="1">
+        <v>9</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>12</v>
@@ -961,16 +1186,25 @@
         <v>13</v>
       </c>
       <c r="C24" s="1">
-        <v>149</v>
+        <v>50</v>
       </c>
       <c r="D24" s="1">
-        <v>477</v>
+        <v>534</v>
       </c>
       <c r="E24" s="1">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="H24" s="1">
+        <v>88</v>
+      </c>
+      <c r="I24" s="1">
+        <v>572</v>
+      </c>
+      <c r="J24" s="1">
+        <v>14</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>13</v>
@@ -990,16 +1224,25 @@
         <v>14</v>
       </c>
       <c r="C25" s="1">
-        <v>73</v>
+        <v>237</v>
       </c>
       <c r="D25" s="1">
-        <v>500</v>
+        <v>546</v>
       </c>
       <c r="E25" s="1">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="H25" s="1">
+        <v>255</v>
+      </c>
+      <c r="I25" s="1">
+        <v>564</v>
+      </c>
+      <c r="J25" s="1">
+        <v>17</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>14</v>
@@ -1019,16 +1262,25 @@
         <v>15</v>
       </c>
       <c r="C26" s="1">
-        <v>50</v>
+        <v>121</v>
       </c>
       <c r="D26" s="1">
-        <v>534</v>
+        <v>336</v>
       </c>
       <c r="E26" s="1">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="H26" s="1">
+        <v>209</v>
+      </c>
+      <c r="I26" s="1">
+        <v>424</v>
+      </c>
+      <c r="J26" s="1">
+        <v>22</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>15</v>
@@ -1048,16 +1300,25 @@
         <v>16</v>
       </c>
       <c r="C27" s="1">
-        <v>237</v>
+        <v>149</v>
       </c>
       <c r="D27" s="1">
-        <v>546</v>
+        <v>477</v>
       </c>
       <c r="E27" s="1">
-        <v>109</v>
+        <v>47</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="H27" s="1">
+        <v>249</v>
+      </c>
+      <c r="I27" s="1">
+        <v>577</v>
+      </c>
+      <c r="J27" s="1">
+        <v>27</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>16</v>
@@ -1077,16 +1338,25 @@
         <v>17</v>
       </c>
       <c r="C28" s="1">
-        <v>276</v>
+        <v>119</v>
       </c>
       <c r="D28" s="1">
-        <v>668</v>
+        <v>428</v>
       </c>
       <c r="E28" s="1">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="H28" s="1">
+        <v>171</v>
+      </c>
+      <c r="I28" s="1">
+        <v>480</v>
+      </c>
+      <c r="J28" s="1">
+        <v>32</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>17</v>
@@ -1116,6 +1386,15 @@
       </c>
       <c r="G29" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="H29" s="1">
+        <v>175.9</v>
+      </c>
+      <c r="I29" s="1">
+        <v>512</v>
+      </c>
+      <c r="J29" s="1">
+        <v>15.8</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>22</v>

</xml_diff>